<commit_message>
output to excel choice
</commit_message>
<xml_diff>
--- a/out.xlsx
+++ b/out.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -551,126 +551,40 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>841040.2447500003</v>
+        <v>504856.049390626</v>
       </c>
       <c r="C3" t="n">
-        <v>1033302.498609375</v>
+        <v>1010532.421640625</v>
       </c>
       <c r="D3" t="n">
-        <v>241286.973375</v>
+        <v>399923.9929531248</v>
       </c>
       <c r="E3" t="n">
-        <v>-15.89597552499997</v>
+        <v>-49.5143950609374</v>
       </c>
       <c r="F3" t="n">
-        <v>-3.264897417545033</v>
+        <v>-4.25731054355469</v>
       </c>
       <c r="G3" t="n">
-        <v>70</v>
+        <v>156</v>
       </c>
       <c r="H3" t="n">
-        <v>44.28571428571428</v>
+        <v>34.61538461538461</v>
       </c>
       <c r="I3" t="n">
-        <v>4.813865009971874</v>
+        <v>6.721220520353199</v>
       </c>
       <c r="J3" t="n">
-        <v>-3.605241126803183</v>
+        <v>-4.439136829842005</v>
       </c>
       <c r="K3" t="n">
-        <v>0.1477733662826219</v>
+        <v>-0.06925583491882437</v>
       </c>
       <c r="L3" s="2" t="n">
-        <v>1.791666666666667</v>
+        <v>1.270833333333333</v>
       </c>
       <c r="M3" s="2" t="n">
-        <v>0.4354166666666667</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>SmaCross</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>841040.2447500003</v>
-      </c>
-      <c r="C4" t="n">
-        <v>1033302.498609375</v>
-      </c>
-      <c r="D4" t="n">
-        <v>241286.973375</v>
-      </c>
-      <c r="E4" t="n">
-        <v>-15.89597552499997</v>
-      </c>
-      <c r="F4" t="n">
-        <v>-3.264897417545033</v>
-      </c>
-      <c r="G4" t="n">
-        <v>70</v>
-      </c>
-      <c r="H4" t="n">
-        <v>44.28571428571428</v>
-      </c>
-      <c r="I4" t="n">
-        <v>4.813865009971874</v>
-      </c>
-      <c r="J4" t="n">
-        <v>-3.605241126803183</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0.1477733662826219</v>
-      </c>
-      <c r="L4" s="2" t="n">
-        <v>1.791666666666667</v>
-      </c>
-      <c r="M4" s="2" t="n">
-        <v>0.4354166666666667</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>EmaCross</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>974364.0074999999</v>
-      </c>
-      <c r="C5" t="n">
-        <v>1070815.13278125</v>
-      </c>
-      <c r="D5" t="n">
-        <v>46924.42343749999</v>
-      </c>
-      <c r="E5" t="n">
-        <v>-2.563599250000005</v>
-      </c>
-      <c r="F5" t="n">
-        <v>-2.044188419442756</v>
-      </c>
-      <c r="G5" t="n">
-        <v>13</v>
-      </c>
-      <c r="H5" t="n">
-        <v>38.46153846153847</v>
-      </c>
-      <c r="I5" t="n">
-        <v>7.036803787379187</v>
-      </c>
-      <c r="J5" t="n">
-        <v>-4.739943076511444</v>
-      </c>
-      <c r="K5" t="n">
-        <v>-0.09891279377823858</v>
-      </c>
-      <c r="L5" s="2" t="n">
-        <v>7.666666666666667</v>
-      </c>
-      <c r="M5" s="2" t="n">
-        <v>1.764583333333333</v>
+        <v>0.1958333333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed Y to y
</commit_message>
<xml_diff>
--- a/out.xlsx
+++ b/out.xlsx
@@ -1,37 +1,93 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\achap\Documents\GitHub\backtesting\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E373B030-9F4A-470F-9E73-874ADAE9E5A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="8430" yWindow="1830" windowWidth="16695" windowHeight="13380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+  <si>
+    <t>Strategy</t>
+  </si>
+  <si>
+    <t>Equity Final [$]</t>
+  </si>
+  <si>
+    <t>Equity Peak [$]</t>
+  </si>
+  <si>
+    <t>Commissions [$]</t>
+  </si>
+  <si>
+    <t>Return [%]</t>
+  </si>
+  <si>
+    <t>Buy &amp; Hold Return [%]</t>
+  </si>
+  <si>
+    <t># Trades</t>
+  </si>
+  <si>
+    <t>Win Rate [%]</t>
+  </si>
+  <si>
+    <t>Best Trade [%]</t>
+  </si>
+  <si>
+    <t>Worst Trade [%]</t>
+  </si>
+  <si>
+    <t>Avg. Trade [%]</t>
+  </si>
+  <si>
+    <t>Max. Trade Duration</t>
+  </si>
+  <si>
+    <t>Avg. Trade Duration</t>
+  </si>
+  <si>
+    <t>EmaCross</t>
+  </si>
+  <si>
+    <t>SmaCross</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,94 +102,44 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -421,169 +427,189 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:M3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Strategy</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Equity Final [$]</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Equity Peak [$]</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Commissions [$]</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Return [%]</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Buy &amp; Hold Return [%]</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t># Trades</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Win Rate [%]</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Best Trade [%]</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Worst Trade [%]</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Avg. Trade [%]</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Max. Trade Duration</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Avg. Trade Duration</t>
-        </is>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>EmaCross</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
         <v>1155771.778515625</v>
       </c>
-      <c r="C2" t="n">
-        <v>1234551.80728125</v>
-      </c>
-      <c r="D2" t="n">
-        <v>81291.03298437501</v>
-      </c>
-      <c r="E2" t="n">
+      <c r="C2">
+        <v>1234551.8072812499</v>
+      </c>
+      <c r="D2">
+        <v>81291.032984375008</v>
+      </c>
+      <c r="E2">
         <v>15.57717785156253</v>
       </c>
-      <c r="F2" t="n">
-        <v>-2.20997640620936</v>
-      </c>
-      <c r="G2" t="n">
+      <c r="F2">
+        <v>-2.2099764062093601</v>
+      </c>
+      <c r="G2">
         <v>19</v>
       </c>
-      <c r="H2" t="n">
-        <v>57.89473684210527</v>
-      </c>
-      <c r="I2" t="n">
-        <v>7.472265629532194</v>
-      </c>
-      <c r="J2" t="n">
+      <c r="H2">
+        <v>57.894736842105267</v>
+      </c>
+      <c r="I2">
+        <v>7.4722656295321936</v>
+      </c>
+      <c r="J2">
         <v>-1.48845119003933</v>
       </c>
-      <c r="K2" t="n">
-        <v>0.9731947980055722</v>
-      </c>
-      <c r="L2" s="2" t="n">
+      <c r="K2">
+        <v>0.97319479800557218</v>
+      </c>
+      <c r="L2" s="2">
         <v>6.427083333333333</v>
       </c>
-      <c r="M2" s="2" t="n">
+      <c r="M2" s="2">
         <v>1.427083333333333</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>SmaCross</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>504856.049390626</v>
-      </c>
-      <c r="C3" t="n">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>504856.04939062602</v>
+      </c>
+      <c r="C3">
         <v>1010532.421640625</v>
       </c>
-      <c r="D3" t="n">
-        <v>399923.9929531248</v>
-      </c>
-      <c r="E3" t="n">
-        <v>-49.5143950609374</v>
-      </c>
-      <c r="F3" t="n">
-        <v>-4.25731054355469</v>
-      </c>
-      <c r="G3" t="n">
+      <c r="D3">
+        <v>399923.99295312481</v>
+      </c>
+      <c r="E3">
+        <v>-49.514395060937403</v>
+      </c>
+      <c r="F3">
+        <v>-4.2573105435546896</v>
+      </c>
+      <c r="G3">
         <v>156</v>
       </c>
-      <c r="H3" t="n">
-        <v>34.61538461538461</v>
-      </c>
-      <c r="I3" t="n">
-        <v>6.721220520353199</v>
-      </c>
-      <c r="J3" t="n">
-        <v>-4.439136829842005</v>
-      </c>
-      <c r="K3" t="n">
-        <v>-0.06925583491882437</v>
-      </c>
-      <c r="L3" s="2" t="n">
+      <c r="H3">
+        <v>34.615384615384613</v>
+      </c>
+      <c r="I3">
+        <v>6.7212205203531994</v>
+      </c>
+      <c r="J3">
+        <v>-4.4391368298420053</v>
+      </c>
+      <c r="K3">
+        <v>-6.9255834918824366E-2</v>
+      </c>
+      <c r="L3" s="2">
         <v>1.270833333333333</v>
       </c>
-      <c r="M3" s="2" t="n">
+      <c r="M3" s="2">
+        <v>0.1958333333333333</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4">
+        <v>504856.04939062602</v>
+      </c>
+      <c r="C4">
+        <v>1010532.421640625</v>
+      </c>
+      <c r="D4">
+        <v>399923.99295312481</v>
+      </c>
+      <c r="E4">
+        <v>-49.514395060937403</v>
+      </c>
+      <c r="F4">
+        <v>-4.2573105435546896</v>
+      </c>
+      <c r="G4">
+        <v>156</v>
+      </c>
+      <c r="H4">
+        <v>34.615384615384613</v>
+      </c>
+      <c r="I4">
+        <v>6.7212205203531994</v>
+      </c>
+      <c r="J4">
+        <v>-4.4391368298420053</v>
+      </c>
+      <c r="K4">
+        <v>-6.9255834918824366E-2</v>
+      </c>
+      <c r="L4" s="2">
+        <v>1.270833333333333</v>
+      </c>
+      <c r="M4" s="2">
         <v>0.1958333333333333</v>
       </c>
     </row>

</xml_diff>

<commit_message>
moved strategies, added time
</commit_message>
<xml_diff>
--- a/out.xlsx
+++ b/out.xlsx
@@ -2,9 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -17,10 +16,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
@@ -37,12 +44,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -55,15 +77,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -426,9 +451,9 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:S6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -452,60 +477,80 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Interval</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Start</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>End</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Duration</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>Equity Final [$]</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Equity Peak [$]</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Commissions [$]</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Return [%]</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Buy &amp; Hold Return [%]</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t># Trades</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Win Rate [%]</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Best Trade [%]</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Worst Trade [%]</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Avg. Trade [%]</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Max. Trade Duration</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Avg. Trade Duration</t>
         </is>
@@ -523,44 +568,330 @@
       <c r="C2" t="n">
         <v>-1</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>15m</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2025/03/01</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2025/03/31</t>
+        </is>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>30.98958333333333</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1160882.784640625</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1240150.96153125</v>
+      </c>
+      <c r="J2" t="n">
+        <v>81635.02685937501</v>
+      </c>
+      <c r="K2" t="n">
+        <v>16.08827846406249</v>
+      </c>
+      <c r="L2" t="n">
+        <v>-2.20997640620936</v>
+      </c>
+      <c r="M2" t="n">
+        <v>19</v>
+      </c>
+      <c r="N2" t="n">
+        <v>57.89473684210527</v>
+      </c>
+      <c r="O2" t="n">
+        <v>7.713160437464572</v>
+      </c>
+      <c r="P2" t="n">
+        <v>-1.498145053841626</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>1.003901241779004</v>
+      </c>
+      <c r="R2" s="2" t="n">
+        <v>6.427083333333333</v>
+      </c>
+      <c r="S2" s="2" t="n">
+        <v>1.427083333333333</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>EmaCross</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>15m</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2025/03/01</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025/03/31</t>
+        </is>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>30.98958333333333</v>
+      </c>
+      <c r="H3" t="n">
         <v>1155771.778515625</v>
       </c>
-      <c r="E2" t="n">
+      <c r="I3" t="n">
         <v>1234551.80728125</v>
       </c>
-      <c r="F2" t="n">
+      <c r="J3" t="n">
         <v>81291.03298437501</v>
       </c>
-      <c r="G2" t="n">
+      <c r="K3" t="n">
         <v>15.57717785156253</v>
       </c>
-      <c r="H2" t="n">
+      <c r="L3" t="n">
         <v>-2.20997640620936</v>
       </c>
-      <c r="I2" t="n">
+      <c r="M3" t="n">
         <v>19</v>
       </c>
-      <c r="J2" t="n">
+      <c r="N3" t="n">
         <v>57.89473684210527</v>
       </c>
-      <c r="K2" t="n">
+      <c r="O3" t="n">
         <v>7.472265629532194</v>
       </c>
-      <c r="L2" t="n">
+      <c r="P3" t="n">
         <v>-1.48845119003933</v>
       </c>
-      <c r="M2" t="n">
+      <c r="Q3" t="n">
         <v>0.9731947980055722</v>
       </c>
-      <c r="N2" s="2" t="n">
+      <c r="R3" s="2" t="n">
         <v>6.427083333333333</v>
       </c>
-      <c r="O2" s="2" t="n">
+      <c r="S3" s="2" t="n">
+        <v>1.427083333333333</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t>EmaCross</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>15m</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2025/03/01</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2025/03/31</t>
+        </is>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>30.98958333333333</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1155771.778515625</v>
+      </c>
+      <c r="I4" t="n">
+        <v>1234551.80728125</v>
+      </c>
+      <c r="J4" t="n">
+        <v>81291.03298437501</v>
+      </c>
+      <c r="K4" t="n">
+        <v>15.57717785156253</v>
+      </c>
+      <c r="L4" t="n">
+        <v>-2.20997640620936</v>
+      </c>
+      <c r="M4" t="n">
+        <v>19</v>
+      </c>
+      <c r="N4" t="n">
+        <v>57.89473684210527</v>
+      </c>
+      <c r="O4" t="n">
+        <v>7.472265629532194</v>
+      </c>
+      <c r="P4" t="n">
+        <v>-1.48845119003933</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0.9731947980055722</v>
+      </c>
+      <c r="R4" s="2" t="n">
+        <v>6.427083333333333</v>
+      </c>
+      <c r="S4" s="2" t="n">
+        <v>1.427083333333333</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>EmaCross</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>15m</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2025/03/01</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2025/03/31</t>
+        </is>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>30.98958333333333</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1155771.778515625</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1234551.80728125</v>
+      </c>
+      <c r="J5" t="n">
+        <v>81291.03298437501</v>
+      </c>
+      <c r="K5" t="n">
+        <v>15.57717785156253</v>
+      </c>
+      <c r="L5" t="n">
+        <v>-2.20997640620936</v>
+      </c>
+      <c r="M5" t="n">
+        <v>19</v>
+      </c>
+      <c r="N5" t="n">
+        <v>57.89473684210527</v>
+      </c>
+      <c r="O5" t="n">
+        <v>7.472265629532194</v>
+      </c>
+      <c r="P5" t="n">
+        <v>-1.48845119003933</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0.9731947980055722</v>
+      </c>
+      <c r="R5" s="2" t="n">
+        <v>6.427083333333333</v>
+      </c>
+      <c r="S5" s="2" t="n">
+        <v>1.427083333333333</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="inlineStr">
+        <is>
+          <t>EmaCross</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>15m</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2025/03/01</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2025/03/31</t>
+        </is>
+      </c>
+      <c r="G6" s="2" t="n">
+        <v>30.98958333333333</v>
+      </c>
+      <c r="H6" t="n">
+        <v>1155771.778515625</v>
+      </c>
+      <c r="I6" t="n">
+        <v>1234551.80728125</v>
+      </c>
+      <c r="J6" t="n">
+        <v>81291.03298437501</v>
+      </c>
+      <c r="K6" t="n">
+        <v>15.57717785156253</v>
+      </c>
+      <c r="L6" t="n">
+        <v>-2.20997640620936</v>
+      </c>
+      <c r="M6" t="n">
+        <v>19</v>
+      </c>
+      <c r="N6" t="n">
+        <v>57.89473684210527</v>
+      </c>
+      <c r="O6" t="n">
+        <v>7.472265629532194</v>
+      </c>
+      <c r="P6" t="n">
+        <v>-1.48845119003933</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0.9731947980055722</v>
+      </c>
+      <c r="R6" s="2" t="n">
+        <v>6.427083333333333</v>
+      </c>
+      <c r="S6" s="2" t="n">
         <v>1.427083333333333</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>